<commit_message>
fixed real traj test
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/tested_state_traj/tested_robot_traj_1_.xlsx
+++ b/dynamics/src/dynamics/tested_state_traj/tested_robot_traj_1_.xlsx
@@ -435,10 +435,10 @@
         <v>1.379316785363834</v>
       </c>
       <c r="E1" t="n">
-        <v>0.188939888900502</v>
+        <v>1.381856437894394</v>
       </c>
       <c r="F1" t="n">
-        <v>-5.725153418012496e-08</v>
+        <v>-1.570796384046431</v>
       </c>
       <c r="G1" t="n">
         <v>-1.367909888287239</v>
@@ -458,10 +458,10 @@
         <v>1.380518500463224</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1878999627744357</v>
+        <v>1.382896364020461</v>
       </c>
       <c r="F2" t="n">
-        <v>-5.762896626571035e-08</v>
+        <v>-1.570796384423863</v>
       </c>
       <c r="G2" t="n">
         <v>-1.322298649847111</v>
@@ -481,10 +481,10 @@
         <v>1.385902980825687</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1832404042758736</v>
+        <v>1.387555922519023</v>
       </c>
       <c r="F3" t="n">
-        <v>-5.932011237774759e-08</v>
+        <v>-1.570796386115009</v>
       </c>
       <c r="G3" t="n">
         <v>-1.117930062140237</v>
@@ -504,10 +504,10 @@
         <v>1.393478433468806</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1766848478679089</v>
+        <v>1.394111478926988</v>
       </c>
       <c r="F4" t="n">
-        <v>-6.169939448241735e-08</v>
+        <v>-1.570796388494291</v>
       </c>
       <c r="G4" t="n">
         <v>-0.8304028629126882</v>
@@ -527,10 +527,10 @@
         <v>1.398862913831269</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1720252893693467</v>
+        <v>1.39877103742555</v>
       </c>
       <c r="F5" t="n">
-        <v>-6.339054059445459e-08</v>
+        <v>-1.570796390185437</v>
       </c>
       <c r="G5" t="n">
         <v>-0.6260342752058142</v>
@@ -550,10 +550,10 @@
         <v>1.40006462893066</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1709853632432805</v>
+        <v>1.399810963551616</v>
       </c>
       <c r="F6" t="n">
-        <v>-6.376797268003997e-08</v>
+        <v>-1.570796390562869</v>
       </c>
       <c r="G6" t="n">
         <v>-0.5804230367656862</v>

</xml_diff>

<commit_message>
fixed real traj data generate
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/tested_state_traj/tested_robot_traj_1_.xlsx
+++ b/dynamics/src/dynamics/tested_state_traj/tested_robot_traj_1_.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,19 +426,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.2028864896758006</v>
+        <v>0.2028864896758006</v>
       </c>
       <c r="C1" t="n">
-        <v>1.56825683117444</v>
+        <v>0.002539495620456482</v>
       </c>
       <c r="D1" t="n">
-        <v>1.379316785363834</v>
+        <v>-1.379316785363834</v>
       </c>
       <c r="E1" t="n">
-        <v>1.381856437894394</v>
+        <v>0.188939888900502</v>
       </c>
       <c r="F1" t="n">
-        <v>-1.570796384046431</v>
+        <v>1.570796384046431</v>
       </c>
       <c r="G1" t="n">
         <v>-1.367909888287239</v>
@@ -446,116 +446,369 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.221347107536837</v>
+        <v>0.2075129133157847</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.2484977296296271</v>
+        <v>0.2046333296544263</v>
       </c>
       <c r="C2" t="n">
-        <v>1.568418617675491</v>
+        <v>0.002533299447576215</v>
       </c>
       <c r="D2" t="n">
-        <v>1.380518500463224</v>
+        <v>-1.379362809194377</v>
       </c>
       <c r="E2" t="n">
-        <v>1.382896364020461</v>
+        <v>0.1889000613375225</v>
       </c>
       <c r="F2" t="n">
-        <v>-1.570796384423863</v>
+        <v>1.570796384060886</v>
       </c>
       <c r="G2" t="n">
-        <v>-1.322298649847111</v>
+        <v>-1.366163048366586</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.4426942150736741</v>
+        <v>0.4150258266315694</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.4528663241188721</v>
+        <v>0.215527422831531</v>
       </c>
       <c r="C3" t="n">
-        <v>1.569143528461966</v>
+        <v>0.002494657279132034</v>
       </c>
       <c r="D3" t="n">
-        <v>1.385902980825687</v>
+        <v>-1.379649834854683</v>
       </c>
       <c r="E3" t="n">
-        <v>1.387555922519023</v>
+        <v>0.1886516784361557</v>
       </c>
       <c r="F3" t="n">
-        <v>-1.570796386115009</v>
+        <v>1.570796384151034</v>
       </c>
       <c r="G3" t="n">
-        <v>-1.117930062140237</v>
+        <v>-1.355268955551023</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.6640413226105111</v>
+        <v>0.6225387399473542</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.7403935328885739</v>
+        <v>0.2412914350012368</v>
       </c>
       <c r="C4" t="n">
-        <v>1.570163409112236</v>
+        <v>0.002403270388835187</v>
       </c>
       <c r="D4" t="n">
-        <v>1.393478433468806</v>
+        <v>-1.380328636888492</v>
       </c>
       <c r="E4" t="n">
-        <v>1.394111478926988</v>
+        <v>0.1880642646891343</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.570796388494291</v>
+        <v>1.570796384364231</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.8304028629126882</v>
+        <v>-1.329504944236346</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.8853884301473481</v>
+        <v>0.8300516532631389</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.9447621273778194</v>
+        <v>0.2844036859956439</v>
       </c>
       <c r="C5" t="n">
-        <v>1.570888319898712</v>
+        <v>0.00225034798971023</v>
       </c>
       <c r="D5" t="n">
-        <v>1.398862913831269</v>
+        <v>-1.381464511358056</v>
       </c>
       <c r="E5" t="n">
-        <v>1.39877103742555</v>
+        <v>0.1870813149555161</v>
       </c>
       <c r="F5" t="n">
-        <v>-1.570796390185437</v>
+        <v>1.570796384720984</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.6260342752058142</v>
+        <v>-1.286392694672704</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1.106735537684185</v>
+        <v>1.037564566578924</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.9903733673316449</v>
+        <v>0.3446388740118342</v>
       </c>
       <c r="C6" t="n">
-        <v>1.571050106399762</v>
+        <v>0.002036689244209476</v>
       </c>
       <c r="D6" t="n">
-        <v>1.40006462893066</v>
+        <v>-1.383051522257715</v>
       </c>
       <c r="E6" t="n">
-        <v>1.399810963551616</v>
+        <v>0.1857079660662958</v>
       </c>
       <c r="F6" t="n">
-        <v>-1.570796390562869</v>
+        <v>1.570796385219429</v>
       </c>
       <c r="G6" t="n">
+        <v>-1.226157508655536</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1.245077479894708</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.4196087999388747</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.001770765274327443</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-1.385026747927482</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.1839986684300178</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.570796385839804</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-1.151187585216519</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1.452590393210493</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.5053030916848213</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.001466801171715305</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-1.387284527466625</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.1820448576383891</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.570796386548922</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-1.065493296314505</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1.660103306526278</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.5966299285037232</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.001142858007795339</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-1.389690707147247</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.1799626260718912</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.57079638730465</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-0.9741664625264626</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1.867616219842062</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.6879567653226248</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0008189148438753735</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-1.392096886827868</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.1778803945053933</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.570796388060378</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-0.8828396287384205</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2.075129133157847</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.7736510570685715</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0005149507412632363</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-1.394354666367011</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.1759265837137646</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1.570796388769496</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-0.7971453398364065</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2.282642046473632</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.8486209829956121</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0002490267713812027</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-1.396329892036778</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.1742172860774866</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1.570796389389871</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-0.7221754163973895</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2.490154959789417</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.908856171011802</v>
+      </c>
+      <c r="C13" t="n">
+        <v>3.536802588044886e-05</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-1.397916902936438</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.1728439371882663</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.570796389888316</v>
+      </c>
+      <c r="G13" t="n">
+        <v>-0.661940230380222</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2.697667873105202</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.9519684220062091</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-0.0001175543732445084</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-1.399052777406001</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.1718609874546481</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1.570796390245069</v>
+      </c>
+      <c r="G14" t="n">
+        <v>-0.6188279808165791</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2.905180786420986</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.9777324341759148</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-0.0002089412635413557</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-1.39973157943981</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.1712735737076268</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1.570796390458266</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-0.5930639695019023</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>3.112693699736771</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.9886265273530191</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-0.0002475834319855381</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-1.400018605100116</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.1710251908062599</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1.570796390548414</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-0.5821698766863396</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>3.320206613052556</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.9903733673316449</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-0.0002537796048658041</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-1.40006462893066</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.1709853632432805</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1.570796390562869</v>
+      </c>
+      <c r="G17" t="n">
         <v>-0.5804230367656862</v>
       </c>
     </row>

</xml_diff>